<commit_message>
Initial Test Cases for Asset Validation & Verification Portal
</commit_message>
<xml_diff>
--- a/docs/qa/matrices/asset-validation.xlsx
+++ b/docs/qa/matrices/asset-validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth\Documents\QA-Journey\CertifyHub-Tests\CertifyHub---Test-Strategy\docs\qa\matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAAC2BA-AEFC-4F64-BC57-F48F5DE94BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5BED9C-6C48-4F33-BCB7-008EB720081B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B6A1F70D-DD27-4DBD-A810-A0A08D366CEF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>TEST CASE ID</t>
   </si>
@@ -68,96 +68,52 @@
     <t>JIRA DEFECT ID(IF THERE IS)</t>
   </si>
   <si>
-    <t>TC10</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>Verify that the system does not leak sensitive admin data.</t>
-  </si>
-  <si>
-    <t>The app will display only the appropriate data for that certificate.</t>
-  </si>
-  <si>
-    <t>1. Go to CertifyHub. (https://certifyhub-api.azurewebsites.net/) 
-2. Locate and Click the "Verify" button. 
-3. Input Valid Certificate ID. 
-4. Click Verify.</t>
-  </si>
-  <si>
-    <t>TC19</t>
-  </si>
-  <si>
-    <t>Verification</t>
-  </si>
-  <si>
-    <t>Verify "Valid/Legit" status is displayed for a genuine certificate.</t>
-  </si>
-  <si>
-    <t>The app confirms the Certifiate is valid.</t>
-  </si>
-  <si>
-    <t>TC20</t>
-  </si>
-  <si>
-    <t>Verify "Invalid" status for a certificate ID that does not exist in DB.</t>
-  </si>
-  <si>
-    <t>The app confirms the Certifiate is invalid.</t>
-  </si>
-  <si>
-    <t>1. Go to CertifyHub. (https://certifyhub-api.azurewebsites.net/) 
-2. Locate and Click the "Verify" button. 
-3. Input invalid Certificate ID. 
-4. Click Verify.</t>
-  </si>
-  <si>
-    <t>TC21</t>
-  </si>
-  <si>
-    <t>Verify "Invalid" status if the URL parameters are manually altered.</t>
-  </si>
-  <si>
-    <t>1. Go to CertifyHub. (https://certifyhub-api.azurewebsites.net/) 
-2. Locate and Click the "Verify" button. 
-3. Input valid Certificate ID. 
-4. Click Verify. 
-5. In the URL address bar alter the ID to something that is random.</t>
-  </si>
-  <si>
-    <t>TC24</t>
-  </si>
-  <si>
-    <t>Verify the verification page displays the correct recipient name.</t>
-  </si>
-  <si>
-    <t>The certificate shows the correct recipient name.</t>
-  </si>
-  <si>
-    <t>1. Go to CertifyHub. (https://certifyhub-api.azurewebsites.net/) 2. Locate and Click the "Verify" button. 3. Input invalid Certificate ID. 4. Click Verify.</t>
-  </si>
-  <si>
-    <t>TC25</t>
-  </si>
-  <si>
-    <t>Verify the verification page displays the correct date of issuance.</t>
-  </si>
-  <si>
-    <t>The certificate shows the correct issuance date.</t>
-  </si>
-  <si>
-    <t>TC32</t>
-  </si>
-  <si>
-    <t>Verify restriction in admin URL while not logged in as Admin</t>
-  </si>
-  <si>
-    <t>The app redirects to login panel.</t>
-  </si>
-  <si>
-    <t>1. Go to CertifyHub. (https://certifyhub-api.azurewebsites.net/)
-2. Go to dashboard route without logging in. (https://certifyhub-api.azurewebsites.net/dashboard)</t>
+    <t>TC16</t>
+  </si>
+  <si>
+    <t>QR Code</t>
+  </si>
+  <si>
+    <t>Verify QR code is clearly visible and not blurred on the generated file.</t>
+  </si>
+  <si>
+    <t>The QR Code is visible and clear.</t>
+  </si>
+  <si>
+    <t>1.  Login as Admin. 
+2. Click "Templates" in the sidebar. 
+3. Click "Reuse" your desired template. 
+4. Upload excel file containing the certificate reciever's appropriate data (Name, email) 
+5. Enable send Certificates.
+6. Click Generate and Send.
+7. Open your inbox and verify. (Also check your spam inbox)</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>Verify QR code scans correctly using a standard mobile camera app.</t>
+  </si>
+  <si>
+    <t>The QR Code is scannable by a mobile camera app.</t>
+  </si>
+  <si>
+    <t>1. Login as Admin. 
+2. Click "Templates" in the sidebar. 
+3. Click "Reuse" your desired template. 
+4. Upload excel file containing the certificate reciever's appropriate data (Name, email) 
+5. Enable send Certificates. 
+6. Click Generate and Send. 
+7. Open your inbox and verify. (Also check your spam inbox)</t>
+  </si>
+  <si>
+    <t>TC18</t>
+  </si>
+  <si>
+    <t>Verify QR code redirects to the correct unique verification URL.</t>
+  </si>
+  <si>
+    <t>The QR Code redirects to the verification Portal of CertifyHub.</t>
   </si>
 </sst>
 </file>
@@ -565,21 +521,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E1D032-4572-4826-B4CD-3DD8E0382E83}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="48" customWidth="1"/>
-    <col min="5" max="5" width="56.5546875" customWidth="1"/>
-    <col min="6" max="6" width="48.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="39" customWidth="1"/>
+    <col min="5" max="5" width="76.6640625" customWidth="1"/>
+    <col min="6" max="6" width="40.33203125" customWidth="1"/>
+    <col min="7" max="7" width="33.77734375" customWidth="1"/>
     <col min="8" max="8" width="22.21875" customWidth="1"/>
     <col min="9" max="9" width="33.21875" customWidth="1"/>
     <col min="10" max="10" width="51.77734375" customWidth="1"/>
@@ -617,7 +573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="106.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -636,117 +592,41 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:10" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:10" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:10" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:10" ht="54" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:10" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:10" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial test Cases for User Side module
</commit_message>
<xml_diff>
--- a/docs/qa/matrices/asset-validation.xlsx
+++ b/docs/qa/matrices/asset-validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth\Documents\QA-Journey\CertifyHub-Tests\CertifyHub---Test-Strategy\docs\qa\matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5BED9C-6C48-4F33-BCB7-008EB720081B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF2A764-3FEC-4E10-9F74-9800D6B2413A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B6A1F70D-DD27-4DBD-A810-A0A08D366CEF}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>